<commit_message>
Update Burndown chart sprint 4
</commit_message>
<xml_diff>
--- a/ScrumDocs/Sprint 4/burndownChart_Sprint_4.xlsx
+++ b/ScrumDocs/Sprint 4/burndownChart_Sprint_4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d12c58815c542ef2/Documentos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleix\Documents\GitHub\ES\ScrumDocs\Sprint 4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="60">
   <si>
     <t>Status</t>
   </si>
@@ -256,6 +256,24 @@
   </si>
   <si>
     <t>Generar dinàmicament els totems dins el GameManager</t>
+  </si>
+  <si>
+    <t>Eliminar fletxa de disparar quan el personatge mor</t>
+  </si>
+  <si>
+    <t>Francisco</t>
+  </si>
+  <si>
+    <t>Francsico</t>
+  </si>
+  <si>
+    <t>Poder assignar un objecte a un personatge a principi de torn</t>
+  </si>
+  <si>
+    <t>Implementar objectes de defensa</t>
+  </si>
+  <si>
+    <t>Implementar objectes de desplaçament</t>
   </si>
 </sst>
 </file>
@@ -430,7 +448,49 @@
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="42">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="43"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -836,7 +896,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -851,7 +911,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>1</c:v>
@@ -860,10 +920,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>4</c:v>
@@ -975,43 +1035,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>83.571428571428569</c:v>
+                  <c:v>107.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>77.142857142857139</c:v>
+                  <c:v>99</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.714285714285722</c:v>
+                  <c:v>90.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>64.285714285714278</c:v>
+                  <c:v>82.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>57.857142857142854</c:v>
+                  <c:v>74.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>51.428571428571431</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45</c:v>
+                  <c:v>57.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38.571428571428569</c:v>
+                  <c:v>49.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32.142857142857146</c:v>
+                  <c:v>41.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.714285714285708</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19.285714285714292</c:v>
+                  <c:v>24.75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12.857142857142861</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.4285714285714306</c:v>
+                  <c:v>8.25</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -1123,40 +1183,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>90</c:v>
+                  <c:v>115.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>58</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45.5</c:v>
+                  <c:v>65.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38.5</c:v>
+                  <c:v>55.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.5</c:v>
+                  <c:v>47.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -1544,46 +1604,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1850,7 +1910,7 @@
         <c:axId val="-1967054272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="26"/>
+          <c:max val="31"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2516,15 +2576,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>143387</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>10242</xdr:rowOff>
+      <xdr:colOff>860323</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>40968</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>425621</xdr:colOff>
-      <xdr:row>70</xdr:row>
-      <xdr:rowOff>112661</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>97879</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>143387</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2908,9 +2968,9 @@
   <dimension ref="A1:AD55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A40" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="9" topLeftCell="A50" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="Q53" sqref="Q53"/>
+      <selection pane="bottomLeft" activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2935,59 +2995,59 @@
       </c>
       <c r="E1" s="2">
         <f>E5</f>
-        <v>90</v>
+        <v>115.5</v>
       </c>
       <c r="F1" s="2">
         <f>E1-F9*E1/14</f>
-        <v>83.571428571428569</v>
+        <v>107.25</v>
       </c>
       <c r="G1" s="2">
         <f>E1-G9*E1/14</f>
-        <v>77.142857142857139</v>
+        <v>99</v>
       </c>
       <c r="H1" s="2">
         <f>E1-H9*E1/14</f>
-        <v>70.714285714285722</v>
+        <v>90.75</v>
       </c>
       <c r="I1" s="2">
         <f>E1-I9*E1/14</f>
-        <v>64.285714285714278</v>
+        <v>82.5</v>
       </c>
       <c r="J1" s="2">
         <f>E1-J9*E1/14</f>
-        <v>57.857142857142854</v>
+        <v>74.25</v>
       </c>
       <c r="K1" s="2">
         <f>E1-K9*E1/14</f>
-        <v>51.428571428571431</v>
+        <v>66</v>
       </c>
       <c r="L1" s="2">
         <f>E1-L9*E1/14</f>
-        <v>45</v>
+        <v>57.75</v>
       </c>
       <c r="M1" s="2">
         <f>E1-M9*E1/14</f>
-        <v>38.571428571428569</v>
+        <v>49.5</v>
       </c>
       <c r="N1" s="2">
         <f>E1-N9*E1/14</f>
-        <v>32.142857142857146</v>
+        <v>41.25</v>
       </c>
       <c r="O1" s="2">
         <f>E1-O9*E1/14</f>
-        <v>25.714285714285708</v>
+        <v>33</v>
       </c>
       <c r="P1" s="2">
         <f>E1-P9*E1/14</f>
-        <v>19.285714285714292</v>
+        <v>24.75</v>
       </c>
       <c r="Q1" s="2">
         <f>E1-Q9*E1/14</f>
-        <v>12.857142857142861</v>
+        <v>16.5</v>
       </c>
       <c r="R1" s="2">
         <f>E1-R9*E1/14</f>
-        <v>6.4285714285714306</v>
+        <v>8.25</v>
       </c>
       <c r="S1" s="2">
         <f>E1-S9*E1/14</f>
@@ -3012,63 +3072,63 @@
         <v>19</v>
       </c>
       <c r="E2" s="2">
-        <f>COUNTIF(E10:E37,0)</f>
+        <f>COUNTIF(E10:E40,0)</f>
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <f>COUNTIF(F10:F37,0)</f>
+        <f>COUNTIF(F10:F40,0)</f>
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <f>COUNTIF(G10:G37,0)</f>
-        <v>8</v>
+        <f>COUNTIF(G10:G40,0)</f>
+        <v>9</v>
       </c>
       <c r="H2" s="2">
-        <f>COUNTIF(H10:H37,0)</f>
+        <f>COUNTIF(H10:H40,0)</f>
         <v>1</v>
       </c>
       <c r="I2" s="2">
-        <f>COUNTIF(I10:I37,0)</f>
+        <f>COUNTIF(I10:I40,0)</f>
         <v>5</v>
       </c>
       <c r="J2" s="2">
-        <f>COUNTIF(J10:J37,0)</f>
+        <f>COUNTIF(J10:J40,0)</f>
         <v>2</v>
       </c>
       <c r="K2" s="2">
-        <f>COUNTIF(K10:K37,0)</f>
+        <f>COUNTIF(K10:K40,0)</f>
         <v>0</v>
       </c>
       <c r="L2" s="2">
-        <f>COUNTIF(L10:L37,0)</f>
-        <v>3</v>
+        <f>COUNTIF(L10:L40,0)</f>
+        <v>4</v>
       </c>
       <c r="M2" s="2">
-        <f>COUNTIF(M10:M37,0)</f>
+        <f>COUNTIF(M10:M40,0)</f>
         <v>1</v>
       </c>
       <c r="N2" s="2">
-        <f>COUNTIF(N10:N37,0)</f>
+        <f>COUNTIF(N10:N40,0)</f>
         <v>0</v>
       </c>
       <c r="O2" s="2">
-        <f>COUNTIF(O10:O37,0)</f>
-        <v>1</v>
+        <f>COUNTIF(O10:O40,0)</f>
+        <v>2</v>
       </c>
       <c r="P2" s="2">
-        <f>COUNTIF(P10:P37,0)</f>
-        <v>1</v>
+        <f>COUNTIF(P10:P40,0)</f>
+        <v>2</v>
       </c>
       <c r="Q2" s="2">
-        <f>COUNTIF(Q10:Q37,0)</f>
+        <f>COUNTIF(Q10:Q40,0)</f>
         <v>4</v>
       </c>
       <c r="R2" s="2">
-        <f>COUNTIF(R10:R37,0)</f>
+        <f>COUNTIF(R10:R40,0)</f>
         <v>0</v>
       </c>
       <c r="S2" s="2">
-        <f>COUNTIF(S10:S37,0)</f>
+        <f>COUNTIF(S10:S40,0)</f>
         <v>0</v>
       </c>
       <c r="T2" s="3"/>
@@ -3090,63 +3150,63 @@
         <v>20</v>
       </c>
       <c r="E3" s="2">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F3" s="2">
         <f>E3-F2</f>
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G3" s="2">
         <f t="shared" ref="G3:S3" si="0">F3-G2</f>
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H3" s="2">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="I3" s="2">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="K3" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="M3" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="N3" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="O3" s="2">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="P3" s="2">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q3" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S3" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3" s="3"/>
       <c r="U3" s="3"/>
@@ -3214,63 +3274,63 @@
         <v>7</v>
       </c>
       <c r="E5" s="10">
-        <f>SUM(E10:E37)</f>
-        <v>90</v>
+        <f>SUM(E10:E40)</f>
+        <v>115.5</v>
       </c>
       <c r="F5" s="10">
-        <f>SUM(F10:F37)</f>
-        <v>90</v>
+        <f>SUM(F10:F40)</f>
+        <v>115.5</v>
       </c>
       <c r="G5" s="10">
-        <f>SUM(G10:G37)</f>
-        <v>60</v>
+        <f>SUM(G10:G40)</f>
+        <v>85</v>
       </c>
       <c r="H5" s="10">
-        <f>SUM(H10:H37)</f>
-        <v>58</v>
+        <f>SUM(H10:H40)</f>
+        <v>81</v>
       </c>
       <c r="I5" s="10">
-        <f>SUM(I10:I37)</f>
-        <v>45.5</v>
+        <f>SUM(I10:I40)</f>
+        <v>65.5</v>
       </c>
       <c r="J5" s="10">
-        <f>SUM(J10:J37)</f>
-        <v>38.5</v>
+        <f>SUM(J10:J40)</f>
+        <v>55.5</v>
       </c>
       <c r="K5" s="10">
-        <f>SUM(K10:K37)</f>
-        <v>35.5</v>
+        <f>SUM(K10:K40)</f>
+        <v>47.5</v>
       </c>
       <c r="L5" s="10">
-        <f>SUM(L10:L37)</f>
-        <v>27</v>
+        <f>SUM(L10:L40)</f>
+        <v>34</v>
       </c>
       <c r="M5" s="10">
-        <f>SUM(M10:M37)</f>
-        <v>23</v>
+        <f>SUM(M10:M40)</f>
+        <v>28</v>
       </c>
       <c r="N5" s="10">
-        <f>SUM(N10:N37)</f>
-        <v>21</v>
+        <f>SUM(N10:N40)</f>
+        <v>24</v>
       </c>
       <c r="O5" s="10">
-        <f>SUM(O10:O37)</f>
+        <f>SUM(O10:O40)</f>
         <v>17</v>
       </c>
       <c r="P5" s="10">
-        <f>SUM(P10:P37)</f>
-        <v>15</v>
+        <f>SUM(P10:P40)</f>
+        <v>12</v>
       </c>
       <c r="Q5" s="10">
-        <f>SUM(Q10:Q37)</f>
-        <v>6</v>
+        <f>SUM(Q10:Q40)</f>
+        <v>3</v>
       </c>
       <c r="R5" s="10">
-        <f>SUM(R10:R37)</f>
+        <f>SUM(R10:R40)</f>
         <v>0</v>
       </c>
       <c r="S5" s="10">
-        <f>SUM(S10:S37)</f>
+        <f>SUM(S10:S40)</f>
         <v>0</v>
       </c>
       <c r="T5" s="13" t="str">
@@ -3329,59 +3389,59 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1">
         <f>IF(F9="","",$E5-$E5/($B4-1)*(F9-1))</f>
-        <v>90</v>
+        <v>115.5</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" ref="G6:AD6" si="2">IF(G9="","",TotalEffort-TotalEffort/(ImplementationDays)*(G9-1))</f>
-        <v>83.571428571428569</v>
+        <v>107.25</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="2"/>
-        <v>77.142857142857139</v>
+        <v>99</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
-        <v>70.714285714285722</v>
+        <v>90.75</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="2"/>
-        <v>64.285714285714278</v>
+        <v>82.5</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
-        <v>57.857142857142854</v>
+        <v>74.25</v>
       </c>
       <c r="L6" s="1">
         <f t="shared" si="2"/>
-        <v>51.428571428571431</v>
+        <v>66</v>
       </c>
       <c r="M6" s="1">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>57.75</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" si="2"/>
-        <v>38.571428571428569</v>
+        <v>49.5</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" si="2"/>
-        <v>32.142857142857139</v>
+        <v>41.25</v>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="2"/>
-        <v>25.714285714285708</v>
+        <v>33</v>
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="2"/>
-        <v>19.285714285714278</v>
+        <v>24.75</v>
       </c>
       <c r="R6" s="1">
         <f t="shared" si="2"/>
-        <v>12.857142857142861</v>
+        <v>16.5</v>
       </c>
       <c r="S6" s="1">
         <f t="shared" si="2"/>
-        <v>6.4285714285714306</v>
+        <v>8.25</v>
       </c>
       <c r="T6" s="14" t="str">
         <f t="shared" si="2"/>
@@ -3439,51 +3499,51 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1">
         <f t="shared" ref="F7:AD7" ca="1" si="3">IF(TREND(OFFSET($F5,0,DoneDays-TrendDays,1,TrendDays),OFFSET($F8,0,DoneDays-TrendDays,1,TrendDays),F8)&lt;0,"",TREND(OFFSET($F5,0,DoneDays-TrendDays,1,TrendDays),OFFSET($F8,0,DoneDays-TrendDays,1,TrendDays),F8))</f>
-        <v>70.865384615384613</v>
+        <v>98.21794871794873</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>64.5944055944056</v>
+        <v>88.966200466200476</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>58.323426573426573</v>
+        <v>79.714452214452223</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>52.052447552447553</v>
+        <v>70.462703962703969</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>45.781468531468533</v>
+        <v>61.210955710955716</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>39.510489510489506</v>
+        <v>51.959207459207462</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>33.239510489510486</v>
+        <v>42.707459207459209</v>
       </c>
       <c r="M7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>26.968531468531467</v>
+        <v>33.455710955710956</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>20.697552447552447</v>
+        <v>24.203962703962702</v>
       </c>
       <c r="O7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>14.426573426573427</v>
+        <v>14.952214452214449</v>
       </c>
       <c r="P7" s="1">
         <f t="shared" ca="1" si="3"/>
-        <v>8.1555944055943996</v>
-      </c>
-      <c r="Q7" s="1">
+        <v>5.7004662004661952</v>
+      </c>
+      <c r="Q7" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>1.8846153846153726</v>
+        <v/>
       </c>
       <c r="R7" s="1" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4969,56 +5029,36 @@
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B34" s="17">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="E34" s="17">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="F34" s="17">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="G34" s="17">
-        <v>3</v>
-      </c>
-      <c r="H34" s="17">
-        <v>3</v>
-      </c>
-      <c r="I34" s="17">
-        <v>3</v>
-      </c>
-      <c r="J34" s="17">
-        <v>3</v>
-      </c>
-      <c r="K34" s="17">
-        <v>3</v>
-      </c>
-      <c r="L34" s="17">
-        <v>3</v>
-      </c>
-      <c r="M34" s="17">
-        <v>3</v>
-      </c>
-      <c r="N34" s="17">
-        <v>3</v>
-      </c>
-      <c r="O34" s="17">
-        <v>3</v>
-      </c>
-      <c r="P34" s="17">
-        <v>3</v>
-      </c>
-      <c r="Q34" s="17">
-        <v>3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="17"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
       <c r="R34" s="17"/>
       <c r="S34" s="17"/>
     </row>
@@ -5190,13 +5230,153 @@
       <c r="S37" s="17"/>
     </row>
     <row r="38" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C38"/>
+      <c r="A38" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="17">
+        <v>92</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="17">
+        <v>15</v>
+      </c>
+      <c r="F38" s="17">
+        <v>15</v>
+      </c>
+      <c r="G38" s="17">
+        <v>15</v>
+      </c>
+      <c r="H38" s="17">
+        <v>15</v>
+      </c>
+      <c r="I38" s="17">
+        <v>12</v>
+      </c>
+      <c r="J38" s="17">
+        <v>12</v>
+      </c>
+      <c r="K38" s="17">
+        <v>7</v>
+      </c>
+      <c r="L38" s="17">
+        <v>7</v>
+      </c>
+      <c r="M38" s="17">
+        <v>5</v>
+      </c>
+      <c r="N38" s="17">
+        <v>3</v>
+      </c>
+      <c r="O38" s="17">
+        <v>0</v>
+      </c>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C39"/>
+      <c r="A39" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B39" s="17">
+        <v>104</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E39" s="17">
+        <v>3</v>
+      </c>
+      <c r="F39" s="17">
+        <v>3</v>
+      </c>
+      <c r="G39" s="17">
+        <v>3</v>
+      </c>
+      <c r="H39" s="17">
+        <v>3</v>
+      </c>
+      <c r="I39" s="17">
+        <v>3</v>
+      </c>
+      <c r="J39" s="17">
+        <v>3</v>
+      </c>
+      <c r="K39" s="17">
+        <v>3</v>
+      </c>
+      <c r="L39" s="17">
+        <v>0</v>
+      </c>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="C40"/>
+      <c r="A40" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="17">
+        <v>93</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E40" s="17">
+        <v>10</v>
+      </c>
+      <c r="F40" s="17">
+        <v>10</v>
+      </c>
+      <c r="G40" s="17">
+        <v>10</v>
+      </c>
+      <c r="H40" s="17">
+        <v>8</v>
+      </c>
+      <c r="I40" s="17">
+        <v>8</v>
+      </c>
+      <c r="J40" s="17">
+        <v>5</v>
+      </c>
+      <c r="K40" s="17">
+        <v>5</v>
+      </c>
+      <c r="L40" s="17">
+        <v>3</v>
+      </c>
+      <c r="M40" s="17">
+        <v>3</v>
+      </c>
+      <c r="N40" s="17">
+        <v>3</v>
+      </c>
+      <c r="O40" s="17">
+        <v>3</v>
+      </c>
+      <c r="P40" s="17">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="17"/>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C41"/>
@@ -5255,143 +5435,167 @@
   </customSheetViews>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="B18:C18 A17:C17 A19:C24 D17:S24 A11:S15 D1:S3">
-    <cfRule type="expression" dxfId="35" priority="116" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="122" stopIfTrue="1">
       <formula>$D1="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="117" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="123" stopIfTrue="1">
       <formula>$D1="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="expression" dxfId="33" priority="91" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="97" stopIfTrue="1">
       <formula>$D11="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="98" stopIfTrue="1">
       <formula>$D11="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D3">
-    <cfRule type="expression" dxfId="31" priority="135" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="141" stopIfTrue="1">
       <formula>$D1048550="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="136" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="142" stopIfTrue="1">
       <formula>$D1048550="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:S26">
-    <cfRule type="expression" dxfId="25" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="35" stopIfTrue="1">
       <formula>$D25="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="36" stopIfTrue="1">
       <formula>$D25="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16:S16">
-    <cfRule type="expression" dxfId="29" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="33" stopIfTrue="1">
       <formula>$D16="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="34" stopIfTrue="1">
       <formula>$D16="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:S10">
-    <cfRule type="expression" dxfId="27" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="31" stopIfTrue="1">
       <formula>$D10="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="32" stopIfTrue="1">
       <formula>$D10="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:S27">
-    <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="29" stopIfTrue="1">
       <formula>$D27="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="30" stopIfTrue="1">
       <formula>$D27="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:S28">
-    <cfRule type="expression" dxfId="21" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="27" stopIfTrue="1">
       <formula>$D28="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="28" stopIfTrue="1">
       <formula>$D28="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:S29">
-    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="25" stopIfTrue="1">
       <formula>$D29="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="26" stopIfTrue="1">
       <formula>$D29="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:S30">
-    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="23" stopIfTrue="1">
       <formula>$D30="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="24" stopIfTrue="1">
       <formula>$D30="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:S31">
-    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="21" stopIfTrue="1">
       <formula>$D31="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="22" stopIfTrue="1">
       <formula>$D31="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:S32">
-    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="19" stopIfTrue="1">
       <formula>$D32="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="20" stopIfTrue="1">
       <formula>$D32="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:S33">
-    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="17" stopIfTrue="1">
       <formula>$D33="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="18" stopIfTrue="1">
       <formula>$D33="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:S34">
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="15" stopIfTrue="1">
       <formula>$D34="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="16" stopIfTrue="1">
       <formula>$D34="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:S35">
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="13" stopIfTrue="1">
       <formula>$D35="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="14" stopIfTrue="1">
       <formula>$D35="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:S36">
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="11" stopIfTrue="1">
       <formula>$D36="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
       <formula>$D36="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:S37">
-    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="7" stopIfTrue="1">
       <formula>$D37="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="8" stopIfTrue="1">
       <formula>$D37="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A38:S38">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
+      <formula>$D38="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
+      <formula>$D38="Ongoing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A39:S39">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
+      <formula>$D39="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
+      <formula>$D39="Ongoing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:S40">
+    <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
+      <formula>$D40="Done"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
+      <formula>$D40="Ongoing"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D1:D3 D10:D37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D1:D3 D10:D40">
       <formula1>"Planned,Ongoing,Done"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Documentació Sprint 4 acabada
</commit_message>
<xml_diff>
--- a/ScrumDocs/Sprint 4/burndownChart_Sprint_4.xlsx
+++ b/ScrumDocs/Sprint 4/burndownChart_Sprint_4.xlsx
@@ -1225,7 +1225,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2971,9 +2971,9 @@
   <dimension ref="A1:AD55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A20" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="G41" sqref="A41:G41"/>
+      <selection pane="bottomLeft" activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3075,63 +3075,63 @@
         <v>19</v>
       </c>
       <c r="E2" s="2">
-        <f>COUNTIF(E10:E41,0)</f>
+        <f t="shared" ref="E2:S2" si="0">COUNTIF(E10:E41,0)</f>
         <v>0</v>
       </c>
       <c r="F2" s="2">
-        <f>COUNTIF(F10:F41,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <f>COUNTIF(G10:G41,0)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="H2" s="2">
-        <f>COUNTIF(H10:H41,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I2" s="2">
-        <f>COUNTIF(I10:I41,0)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="J2" s="2">
-        <f>COUNTIF(J10:J41,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K2" s="2">
-        <f>COUNTIF(K10:K41,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L2" s="2">
-        <f>COUNTIF(L10:L41,0)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="M2" s="2">
-        <f>COUNTIF(M10:M41,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N2" s="2">
-        <f>COUNTIF(N10:N41,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="O2" s="2">
-        <f>COUNTIF(O10:O41,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="P2" s="2">
-        <f>COUNTIF(P10:P41,0)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="Q2" s="2">
-        <f>COUNTIF(Q10:Q41,0)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="R2" s="2">
-        <f>COUNTIF(R10:R41,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="S2" s="2">
-        <f>COUNTIF(S10:S41,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="T2" s="3"/>
@@ -3160,55 +3160,55 @@
         <v>32</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:S3" si="0">F3-G2</f>
+        <f t="shared" ref="G3:S3" si="1">F3-G2</f>
         <v>23</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="N3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="O3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="P3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="Q3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="S3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="T3" s="3"/>
@@ -3277,99 +3277,99 @@
         <v>7</v>
       </c>
       <c r="E5" s="10">
-        <f>SUM(E10:E41)</f>
+        <f t="shared" ref="E5:S5" si="2">SUM(E10:E41)</f>
         <v>119.5</v>
       </c>
       <c r="F5" s="10">
-        <f>SUM(F10:F41)</f>
+        <f t="shared" si="2"/>
         <v>119.5</v>
       </c>
       <c r="G5" s="10">
-        <f>SUM(G10:G41)</f>
+        <f t="shared" si="2"/>
         <v>89</v>
       </c>
       <c r="H5" s="10">
-        <f>SUM(H10:H41)</f>
+        <f t="shared" si="2"/>
         <v>85</v>
       </c>
       <c r="I5" s="10">
-        <f>SUM(I10:I41)</f>
+        <f t="shared" si="2"/>
         <v>65.5</v>
       </c>
       <c r="J5" s="10">
-        <f>SUM(J10:J41)</f>
+        <f t="shared" si="2"/>
         <v>55.5</v>
       </c>
       <c r="K5" s="10">
-        <f>SUM(K10:K41)</f>
+        <f t="shared" si="2"/>
         <v>47.5</v>
       </c>
       <c r="L5" s="10">
-        <f>SUM(L10:L41)</f>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="M5" s="10">
-        <f>SUM(M10:M41)</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="N5" s="10">
-        <f>SUM(N10:N41)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="O5" s="10">
-        <f>SUM(O10:O41)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="P5" s="10">
-        <f>SUM(P10:P41)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="Q5" s="10">
-        <f>SUM(Q10:Q41)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="R5" s="10">
-        <f>SUM(R10:R41)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="S5" s="10">
-        <f>SUM(S10:S41)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="T5" s="13" t="str">
-        <f t="shared" ref="T5:AB5" ca="1" si="1">IF(AND(SUM(OFFSET(T9,1,0,TaskRows,1))=0),"",SUM(OFFSET(T9,1,0,TaskRows,1)))</f>
+        <f t="shared" ref="T5:AB5" ca="1" si="3">IF(AND(SUM(OFFSET(T9,1,0,TaskRows,1))=0),"",SUM(OFFSET(T9,1,0,TaskRows,1)))</f>
         <v/>
       </c>
       <c r="U5" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="V5" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="W5" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="X5" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="Y5" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="Z5" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="AA5" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="AB5" s="13" t="str">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
       <c r="AC5" s="13"/>
@@ -3387,7 +3387,7 @@
       </c>
       <c r="D6" s="1">
         <f ca="1">IF(COUNTIF(F5:AD5,"&gt;0")=0,1,COUNTIF(F5:AD5,"&gt;0"))</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
@@ -3395,99 +3395,99 @@
         <v>119.5</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" ref="G6:AD6" si="2">IF(G9="","",TotalEffort-TotalEffort/(ImplementationDays)*(G9-1))</f>
+        <f t="shared" ref="G6:AD6" si="4">IF(G9="","",TotalEffort-TotalEffort/(ImplementationDays)*(G9-1))</f>
         <v>110.96428571428571</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>102.42857142857143</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>93.892857142857139</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>85.357142857142861</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>76.821428571428569</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>68.285714285714278</v>
       </c>
       <c r="M6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>59.749999999999993</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>51.214285714285708</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>42.678571428571416</v>
       </c>
       <c r="P6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>34.142857142857139</v>
       </c>
       <c r="Q6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>25.607142857142847</v>
       </c>
       <c r="R6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>17.071428571428555</v>
       </c>
       <c r="S6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.5357142857142776</v>
       </c>
       <c r="T6" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="U6" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="V6" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="W6" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="X6" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Y6" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="Z6" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AA6" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AB6" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AC6" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="AD6" s="14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -3501,103 +3501,103 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
-        <f t="shared" ref="F7:AD7" ca="1" si="3">IF(TREND(OFFSET($F5,0,DoneDays-TrendDays,1,TrendDays),OFFSET($F8,0,DoneDays-TrendDays,1,TrendDays),F8)&lt;0,"",TREND(OFFSET($F5,0,DoneDays-TrendDays,1,TrendDays),OFFSET($F8,0,DoneDays-TrendDays,1,TrendDays),F8))</f>
-        <v>99.208791208791183</v>
+        <f t="shared" ref="F7:AD7" ca="1" si="5">IF(TREND(OFFSET($F5,0,DoneDays-TrendDays,1,TrendDays),OFFSET($F8,0,DoneDays-TrendDays,1,TrendDays),F8)&lt;0,"",TREND(OFFSET($F5,0,DoneDays-TrendDays,1,TrendDays),OFFSET($F8,0,DoneDays-TrendDays,1,TrendDays),F8))</f>
+        <v>96.742857142857147</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>90.148351648351635</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>88.298901098901098</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>81.087912087912073</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>79.854945054945063</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>72.027472527472526</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>71.410989010989013</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v>62.967032967032964</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>53.906593406593402</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>54.523076923076921</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>44.846153846153847</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>46.079120879120879</v>
       </c>
       <c r="M7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>35.785714285714292</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>37.635164835164829</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>26.72527472527473</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>29.19120879120878</v>
       </c>
       <c r="O7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>17.664835164835182</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>20.74725274725273</v>
       </c>
       <c r="P7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>8.60439560439562</v>
-      </c>
-      <c r="Q7" s="1" t="str">
-        <f t="shared" ca="1" si="3"/>
-        <v/>
+        <f t="shared" ca="1" si="5"/>
+        <v>12.303296703296695</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>3.8593406593406456</v>
       </c>
       <c r="R7" s="1" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="S7" s="1" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="T7" s="14" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="U7" s="14" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="V7" s="14" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="W7" s="14" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="X7" s="14" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="Y7" s="14" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="Z7" s="14" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AA7" s="14" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AB7" s="14" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AC7" s="14" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
       <c r="AD7" s="14" t="str">
-        <f t="shared" ca="1" si="3"/>
+        <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
     </row>
@@ -3610,7 +3610,7 @@
       </c>
       <c r="D8" s="1">
         <f ca="1">IF(DoneDays&gt;B5,B5,DoneDays)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
@@ -3710,95 +3710,95 @@
         <v>1</v>
       </c>
       <c r="G9" s="11">
-        <f t="shared" ref="G9:AC9" si="4">IF($B$4&gt;F9,F9+1,"")</f>
+        <f t="shared" ref="G9:AC9" si="6">IF($B$4&gt;F9,F9+1,"")</f>
         <v>2</v>
       </c>
       <c r="H9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="I9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="J9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="K9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="L9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="M9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="N9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="O9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="P9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="Q9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>12</v>
       </c>
       <c r="R9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="S9" s="11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="T9" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="U9" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="V9" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="W9" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="X9" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Y9" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="Z9" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AA9" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AB9" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AC9" s="13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="AD9" s="13"/>
@@ -4169,11 +4169,11 @@
       <c r="AA16" s="8"/>
       <c r="AB16" s="8"/>
       <c r="AC16" s="8" t="str">
-        <f t="shared" ref="AC16:AD18" si="5">IF(OR(AC$9="",$E13=""),"",AB16)</f>
+        <f t="shared" ref="AC16:AD18" si="7">IF(OR(AC$9="",$E13=""),"",AB16)</f>
         <v/>
       </c>
       <c r="AD16" s="8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -4221,11 +4221,11 @@
       <c r="AA17" s="8"/>
       <c r="AB17" s="8"/>
       <c r="AC17" s="8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AD17" s="8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -4273,11 +4273,11 @@
       <c r="AA18" s="8"/>
       <c r="AB18" s="8"/>
       <c r="AC18" s="8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="AD18" s="8" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
@@ -4331,11 +4331,11 @@
       <c r="AA19" s="8"/>
       <c r="AB19" s="8"/>
       <c r="AC19" s="8" t="str">
-        <f t="shared" ref="AC19:AD23" si="6">IF(OR(AC$9="",$E20=""),"",AB19)</f>
+        <f t="shared" ref="AC19:AD23" si="8">IF(OR(AC$9="",$E20=""),"",AB19)</f>
         <v/>
       </c>
       <c r="AD19" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -4395,11 +4395,11 @@
       <c r="AA20" s="8"/>
       <c r="AB20" s="8"/>
       <c r="AC20" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD20" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -4447,11 +4447,11 @@
       <c r="AA21" s="8"/>
       <c r="AB21" s="8"/>
       <c r="AC21" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD21" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -4503,11 +4503,11 @@
       <c r="AA22" s="8"/>
       <c r="AB22" s="8"/>
       <c r="AC22" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD22" s="8" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -4546,11 +4546,11 @@
       <c r="R23" s="17"/>
       <c r="S23" s="17"/>
       <c r="AC23" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD23" s="2" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
     </row>
@@ -5030,7 +5030,9 @@
       <c r="R33" s="17">
         <v>3</v>
       </c>
-      <c r="S33" s="17"/>
+      <c r="S33" s="17">
+        <v>3</v>
+      </c>
     </row>
     <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">

</xml_diff>